<commit_message>
Iteration4: Code on CodeSandbox. Paperwork done
</commit_message>
<xml_diff>
--- a/Iteration4/After Coding/defect_log-Iteration3.xlsx
+++ b/Iteration4/After Coding/defect_log-Iteration3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration3\After Coding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive - Ara Institute of Canterbury\Year 2\Semester 1\Software Engineering\Assignment 1\Iteration4\After Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D4C9AE-0241-45C4-8119-13EE97D3145C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6517F174-FC72-4906-87AD-CDDFC02A0BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
   <si>
     <t>PSP Defect Recording Log</t>
   </si>
@@ -653,6 +653,21 @@
   </si>
   <si>
     <t>"Error compiling template" - failed to wrap templates in &lt;div&gt;</t>
+  </si>
+  <si>
+    <t>[Vue warn]: Property or method "tryLower" is not defined on the instance but referenced during render. Make sure that this property is reactive, either in the data option, or for class-based components, by initializing the property. See: https://vuejs.org/v2/guide/reactivity.html#Declaring-Reactive-Properties. - Failed to declare function in props</t>
+  </si>
+  <si>
+    <t>SyntaxError: /src/App.vue: Unterminated string constant (223:11)</t>
+  </si>
+  <si>
+    <t>Random number would remain the same throughout testing, as well as highestNumber/lowestNumber. Added reset function to clear everything</t>
+  </si>
+  <si>
+    <t>[Vue warn]: Invalid prop: type check failed for prop "currentStatement". Expected String with value "78", got Number with value 78. - .toString() added</t>
+  </si>
+  <si>
+    <t>[Vue warn]: Invalid prop: type check failed for prop "currentStatement". Expected String with value "82", got Number with value 82. - .toString() added</t>
   </si>
 </sst>
 </file>
@@ -1311,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,20 +1784,135 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="6"/>
+    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
+        <v>43583</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>16</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="6"/>
+      <c r="A23" s="18">
+        <v>43583</v>
+      </c>
+      <c r="B23">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>17</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <v>43583</v>
+      </c>
+      <c r="B24">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>18</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>43583</v>
+      </c>
+      <c r="B25">
+        <v>19</v>
+      </c>
+      <c r="C25">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>19</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
+        <v>43583</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>70</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>20</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H27" s="6"/>

</xml_diff>